<commit_message>
Roll, pitch, yaw function fixed acordingly data in LITERATURE folder
</commit_message>
<xml_diff>
--- a/data/car_aftercalib_test.xlsx
+++ b/data/car_aftercalib_test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00ce658af401016e/Рабочий стол/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\!PY\RPi_car1.0_soft\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{EB60D934-2EFF-4001-939D-477D968C55D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BC62D81-2321-4F40-8316-63774D16D368}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAC57FB7-8596-4B94-A44C-6802439FA824}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -87,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,6 +152,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1283,6 +1283,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1290,7 +1291,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1340,6 +1340,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2458,6 +2459,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2465,7 +2467,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2515,6 +2516,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3633,6 +3635,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3640,7 +3643,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3690,6 +3692,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3703,13 +3706,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -3750,13 +3759,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -4689,6 +4704,7 @@
         <c:axId val="539731344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4696,9 +4712,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -4713,12 +4729,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4729,9 +4743,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4743,8 +4756,9 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="539735184"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-200"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="539735184"/>
@@ -4757,9 +4771,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -4775,12 +4789,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4791,9 +4803,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4818,6 +4829,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4825,20 +4837,30 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -6569,62 +6591,66 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -6633,9 +6659,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6654,14 +6679,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -6670,20 +6687,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -6692,13 +6709,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6710,30 +6727,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6749,21 +6767,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6782,14 +6797,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6801,14 +6815,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -6822,9 +6836,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6838,12 +6851,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -6855,9 +6862,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6872,14 +6879,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -6891,14 +6897,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -6910,14 +6916,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -6926,14 +6931,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -6941,7 +6945,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -6954,11 +6958,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6966,14 +6978,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6985,12 +6997,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -7006,7 +7025,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -7015,9 +7034,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -7033,14 +7051,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7049,20 +7066,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -7074,12 +7088,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -7088,16 +7096,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>155574</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1494</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>412936</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7124,16 +7132,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>593724</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>595406</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176493</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>317313</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>157443</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7160,16 +7168,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>606424</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>567204</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>143622</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>409761</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>124572</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7196,16 +7204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7531,19 +7539,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EBD2288-6DF5-496F-96EF-21D009C58D3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA40" sqref="AA40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7581,7 +7589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -7620,7 +7628,7 @@
         <v>172.02730121327912</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -7659,7 +7667,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -7698,7 +7706,7 @@
         <v>173.42013977037453</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -7737,7 +7745,7 @@
         <v>-176.90432533815292</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -7776,7 +7784,7 @@
         <v>179.43988898950491</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7815,7 +7823,7 @@
         <v>162.10845334651134</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7854,7 +7862,7 @@
         <v>151.10153574297308</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -7893,7 +7901,7 @@
         <v>142.89537798956115</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -7932,7 +7940,7 @@
         <v>134.69009281825916</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7971,7 +7979,7 @@
         <v>123.60875813633972</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8010,7 +8018,7 @@
         <v>120.33284524158925</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -8049,7 +8057,7 @@
         <v>107.99043897964592</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -8088,7 +8096,7 @@
         <v>101.88684040010483</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -8127,7 +8135,7 @@
         <v>97.126447485430262</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -8166,7 +8174,7 @@
         <v>95.841559835341343</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -8205,7 +8213,7 @@
         <v>103.04045787712285</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -8244,7 +8252,7 @@
         <v>-172.10023746839437</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -8283,7 +8291,7 @@
         <v>-152.12301615715032</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -8322,7 +8330,7 @@
         <v>-154.13352533615625</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -8361,7 +8369,7 @@
         <v>-142.1850081496313</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -8400,7 +8408,7 @@
         <v>-171.08497455694126</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -8439,7 +8447,7 @@
         <v>170.61443343076772</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -8478,7 +8486,7 @@
         <v>-179.3939408339767</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -8517,7 +8525,7 @@
         <v>172.09469179108206</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -8556,7 +8564,7 @@
         <v>152.63958311217905</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -8595,7 +8603,7 @@
         <v>149.02406133284427</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -8634,7 +8642,7 @@
         <v>136.72858148940736</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -8673,7 +8681,7 @@
         <v>128.8701560738503</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -8712,7 +8720,7 @@
         <v>123.1937463378853</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -8751,7 +8759,7 @@
         <v>113.17258697976862</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -8790,7 +8798,7 @@
         <v>105.9484774106506</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -8829,7 +8837,7 @@
         <v>99.962239378509295</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -8868,7 +8876,7 @@
         <v>97.392478991811572</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -8907,7 +8915,7 @@
         <v>96.391882898742935</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -8946,7 +8954,7 @@
         <v>120.2006441618957</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -8985,7 +8993,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -9024,7 +9032,7 @@
         <v>-143.97888202230857</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -9063,7 +9071,7 @@
         <v>-150.54262074074467</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -9102,7 +9110,7 @@
         <v>-141.67711225313664</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -9141,7 +9149,7 @@
         <v>-178.93614305164692</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -9180,7 +9188,7 @@
         <v>170.15288474141437</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -9219,7 +9227,7 @@
         <v>-176.10837053048812</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -9258,7 +9266,7 @@
         <v>167.01766443750964</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -9297,7 +9305,7 @@
         <v>149.20991318122151</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -9336,7 +9344,7 @@
         <v>144.18012516031362</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -9375,7 +9383,7 @@
         <v>135.57316251380641</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -9414,7 +9422,7 @@
         <v>126.00714832239025</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -9453,7 +9461,7 @@
         <v>119.57750623526232</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -9492,7 +9500,7 @@
         <v>109.05425327340055</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -9531,7 +9539,7 @@
         <v>101.07814932551818</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -9570,7 +9578,7 @@
         <v>99.962239378509295</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -9609,7 +9617,7 @@
         <v>96.105663967020305</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -9648,7 +9656,7 @@
         <v>99.731281122191447</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -9687,7 +9695,7 @@
         <v>136.22441568046614</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -9726,7 +9734,7 @@
         <v>-147.22510442149684</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -9765,7 +9773,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -9804,7 +9812,7 @@
         <v>-152.85802485783728</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -9843,7 +9851,7 @@
         <v>-155.80443526020747</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -9882,7 +9890,7 @@
         <v>163.76627255222951</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -9921,7 +9929,7 @@
         <v>165.93391562464271</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -9960,7 +9968,7 @@
         <v>178.71843103188786</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -9999,7 +10007,7 @@
         <v>161.88503960635876</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -10038,7 +10046,7 @@
         <v>148.91108949959687</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -10077,7 +10085,7 @@
         <v>139.47517143312484</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -10116,7 +10124,7 @@
         <v>134.4463353609016</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -10155,7 +10163,7 @@
         <v>126.46627376051683</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -10194,7 +10202,7 @@
         <v>116.39670395624299</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -10233,7 +10241,7 @@
         <v>106.70295642163384</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -10272,7 +10280,7 @@
         <v>101.39610741718678</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -10311,7 +10319,7 @@
         <v>95.613673783205186</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -10350,7 +10358,7 @@
         <v>99.525103425701303</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -10389,7 +10397,7 @@
         <v>105.11166414113953</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -10428,7 +10436,7 @@
         <v>134.72000438181371</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -10467,7 +10475,7 @@
         <v>-135.63497153298019</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -10506,7 +10514,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -10545,7 +10553,7 @@
         <v>-144.11543632235447</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -10584,7 +10592,7 @@
         <v>-154.25085465545828</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -10623,7 +10631,7 @@
         <v>153.69977619196425</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -10662,7 +10670,7 @@
         <v>-176.5955765146883</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -10701,7 +10709,7 @@
         <v>173.03361443304405</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -10740,7 +10748,7 @@
         <v>155.24618944321574</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -10779,7 +10787,7 @@
         <v>143.93296115031191</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -10818,7 +10826,7 @@
         <v>132.96628216004078</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -10857,7 +10865,7 @@
         <v>128.53466625513613</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -10896,7 +10904,7 @@
         <v>119.52043715438904</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -10935,7 +10943,7 @@
         <v>115.2586267479841</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -10974,7 +10982,7 @@
         <v>113.17323982665332</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -11013,7 +11021,7 @@
         <v>109.25831965661953</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -11052,7 +11060,7 @@
         <v>103.96757548063384</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -11091,7 +11099,7 @@
         <v>102.97767129259636</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -11130,7 +11138,7 @@
         <v>96.284062877303697</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -11169,7 +11177,7 @@
         <v>96.355474786464725</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -11208,7 +11216,7 @@
         <v>103.49975575816866</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -11247,7 +11255,7 @@
         <v>122.97723932869681</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -11286,7 +11294,7 @@
         <v>178.41330430697599</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -11325,7 +11333,7 @@
         <v>-147.1466801320735</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -11364,7 +11372,7 @@
         <v>-154.9471710085279</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -11403,7 +11411,7 @@
         <v>-152.16857509502532</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -11442,7 +11450,7 @@
         <v>-168.82614573756589</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -11481,7 +11489,7 @@
         <v>151.12943307069466</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -11520,7 +11528,7 @@
         <v>159.40049306277078</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -11559,7 +11567,7 @@
         <v>165.02060299760726</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -11598,7 +11606,7 @@
         <v>166.32921410779429</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -11637,7 +11645,7 @@
         <v>167.01766443750964</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -11676,7 +11684,7 @@
         <v>155.08347817016059</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -11715,7 +11723,7 @@
         <v>150.20974455615431</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -11754,7 +11762,7 @@
         <v>147.83840518236488</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -11793,7 +11801,7 @@
         <v>149.36496851028076</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -11832,7 +11840,7 @@
         <v>146.65285256260634</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>13</v>
       </c>
@@ -11871,7 +11879,7 @@
         <v>142.46673358364129</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -11910,7 +11918,7 @@
         <v>141.06475895076591</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -11949,7 +11957,7 @@
         <v>143.56005932043317</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -11988,7 +11996,7 @@
         <v>136.89379414891192</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -12027,7 +12035,7 @@
         <v>134.4627707694633</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -12066,7 +12074,7 @@
         <v>135.57316251380641</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -12105,7 +12113,7 @@
         <v>136.87451307009468</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -12144,7 +12152,7 @@
         <v>137.97263923461395</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -12183,7 +12191,7 @@
         <v>136.0799685739843</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -12222,7 +12230,7 @@
         <v>140.55351015486522</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -12261,7 +12269,7 @@
         <v>137.17327625708495</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -12300,7 +12308,7 @@
         <v>134.42699942348682</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -12339,7 +12347,7 @@
         <v>133.24075193442721</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -12378,7 +12386,7 @@
         <v>137.17327625708495</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -12417,7 +12425,7 @@
         <v>137.8591586178828</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -12456,7 +12464,7 @@
         <v>137.39321204175624</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -12495,7 +12503,7 @@
         <v>137.31672962860006</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -12534,7 +12542,7 @@
         <v>133.87222866644063</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>13</v>
       </c>
@@ -12573,7 +12581,7 @@
         <v>132.18220787231127</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -12612,7 +12620,7 @@
         <v>135.94479441011953</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>13</v>
       </c>
@@ -12651,7 +12659,7 @@
         <v>137.17135041995118</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -12690,7 +12698,7 @@
         <v>136.45000790078876</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -12729,7 +12737,7 @@
         <v>137.67319253580823</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -12768,7 +12776,7 @@
         <v>132.99090459811123</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -12807,7 +12815,7 @@
         <v>130.60703976134846</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -12846,7 +12854,7 @@
         <v>120.77011716613391</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -12885,7 +12893,7 @@
         <v>113.35178664784225</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -12924,7 +12932,7 @@
         <v>108.51308097734616</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -12963,7 +12971,7 @@
         <v>100.91845261527155</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -13002,7 +13010,7 @@
         <v>99.409372958709426</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -13041,7 +13049,7 @@
         <v>98.782750354088506</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -13080,7 +13088,7 @@
         <v>108.92873139154878</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -13119,7 +13127,7 @@
         <v>145.10800668002807</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -13158,7 +13166,7 @@
         <v>-146.59143933155664</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -13197,7 +13205,7 @@
         <v>-151.31649944327097</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -13236,7 +13244,7 @@
         <v>-154.42092355526901</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -13275,7 +13283,7 @@
         <v>-165.96649201441664</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -13314,7 +13322,7 @@
         <v>172.23719457114214</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -13353,7 +13361,7 @@
         <v>163.9915304523017</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -13392,7 +13400,7 @@
         <v>175.83124045758728</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -13431,7 +13439,7 @@
         <v>158.52973874881789</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -13470,7 +13478,7 @@
         <v>144.63617985882863</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -13509,7 +13517,7 @@
         <v>137.8591586178828</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -13548,7 +13556,7 @@
         <v>127.79924700859024</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -13587,7 +13595,7 @@
         <v>122.00306617900189</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -13626,7 +13634,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -13665,7 +13673,7 @@
         <v>109.84379643417587</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -13704,7 +13712,7 @@
         <v>101.7168661184463</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -13743,7 +13751,7 @@
         <v>100.31561755392732</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -13782,7 +13790,7 @@
         <v>96.139505273081625</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -13821,7 +13829,7 @@
         <v>101.14761224277018</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -13860,7 +13868,7 @@
         <v>137.07895595975404</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -13899,7 +13907,7 @@
         <v>-160.01679704569509</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -13938,7 +13946,7 @@
         <v>-145.71576563145601</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>11</v>
       </c>
@@ -13977,7 +13985,7 @@
         <v>-151.24497374933287</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -14016,7 +14024,7 @@
         <v>-158.00386912681921</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -14055,7 +14063,7 @@
         <v>167.24102064680005</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -14094,7 +14102,7 @@
         <v>168.56114841014977</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -14133,7 +14141,7 @@
         <v>178.18916776819782</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -14172,7 +14180,7 @@
         <v>158.6841724289111</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -14211,7 +14219,7 @@
         <v>146.91393296095873</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -14250,7 +14258,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -14289,7 +14297,7 @@
         <v>132.58061354586346</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -14328,7 +14336,7 @@
         <v>124.50123123656655</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -14367,7 +14375,7 @@
         <v>116.93626309247912</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -14406,7 +14414,7 @@
         <v>110.43005116310192</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -14445,7 +14453,7 @@
         <v>102.16385965311845</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -14484,7 +14492,7 @@
         <v>98.533239898652084</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -14523,7 +14531,7 @@
         <v>97.596099324924324</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -14562,7 +14570,7 @@
         <v>102.74330458641184</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -14601,7 +14609,7 @@
         <v>140.97504155235538</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -14640,7 +14648,7 @@
         <v>-148.53048361459349</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -14679,7 +14687,7 @@
         <v>-137.80435641277143</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -14718,7 +14726,7 @@
         <v>-143.31403901416189</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -14757,7 +14765,7 @@
         <v>-149.67436028780304</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -14796,7 +14804,7 @@
         <v>154.73767271889207</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -14835,7 +14843,7 @@
         <v>171.44825456630699</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -14874,7 +14882,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -14913,7 +14921,7 @@
         <v>160.58415488866501</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -14952,7 +14960,7 @@
         <v>150.5013414004741</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -14991,7 +14999,7 @@
         <v>142.82402160531819</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -15030,7 +15038,7 @@
         <v>135.42933499982308</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -15069,7 +15077,7 @@
         <v>123.21193440788608</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>11</v>
       </c>
@@ -15108,7 +15116,7 @@
         <v>118.8147979161844</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>11</v>
       </c>
@@ -15147,7 +15155,7 @@
         <v>114.07499133958052</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>11</v>
       </c>
@@ -15186,7 +15194,7 @@
         <v>105.27610814573464</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -15225,7 +15233,7 @@
         <v>99.364860349526865</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -15264,7 +15272,7 @@
         <v>100.76661016842857</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>11</v>
       </c>
@@ -15303,7 +15311,7 @@
         <v>94.602612184824423</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>11</v>
       </c>
@@ -15342,7 +15350,7 @@
         <v>99.243255623325339</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>11</v>
       </c>
@@ -15381,7 +15389,7 @@
         <v>161.18067545795998</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -15420,7 +15428,7 @@
         <v>-148.89468064933351</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -15459,7 +15467,7 @@
         <v>-140.91224917229789</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -15498,7 +15506,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>11</v>
       </c>
@@ -15537,7 +15545,7 @@
         <v>-147.39542688308657</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -15576,7 +15584,7 @@
         <v>179.16477543728095</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>11</v>
       </c>
@@ -15615,7 +15623,7 @@
         <v>162.55907660431578</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -15654,7 +15662,7 @@
         <v>170.98435447122927</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>11</v>
       </c>
@@ -15693,7 +15701,7 @@
         <v>158.03390564628276</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>11</v>
       </c>
@@ -15732,7 +15740,7 @@
         <v>144.988037680037</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -15771,7 +15779,7 @@
         <v>135.9001616975273</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>11</v>
       </c>
@@ -15810,7 +15818,7 @@
         <v>129.01216817031946</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>11</v>
       </c>
@@ -15849,7 +15857,7 @@
         <v>119.1730021979031</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>11</v>
       </c>
@@ -15888,7 +15896,7 @@
         <v>113.41065442357768</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>11</v>
       </c>
@@ -15927,7 +15935,7 @@
         <v>110.66223165060292</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>11</v>
       </c>
@@ -15966,7 +15974,7 @@
         <v>105.09157965710838</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>11</v>
       </c>
@@ -16005,7 +16013,7 @@
         <v>101.39090780537381</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -16044,7 +16052,7 @@
         <v>97.862250052722018</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>11</v>
       </c>
@@ -16083,7 +16091,7 @@
         <v>96.444366043449506</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -16122,7 +16130,7 @@
         <v>110.27105611508546</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>11</v>
       </c>
@@ -16161,7 +16169,7 @@
         <v>135.23238802654225</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>11</v>
       </c>
@@ -16200,7 +16208,7 @@
         <v>174.51271911061292</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>11</v>
       </c>
@@ -16239,7 +16247,7 @@
         <v>-150.5589408209141</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>11</v>
       </c>
@@ -16278,7 +16286,7 @@
         <v>-150.65826943662438</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>11</v>
       </c>
@@ -16317,7 +16325,7 @@
         <v>-147.29056453120242</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>11</v>
       </c>
@@ -16356,7 +16364,7 @@
         <v>-159.82772225189439</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>11</v>
       </c>
@@ -16395,7 +16403,7 @@
         <v>158.15277488507527</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>11</v>
       </c>
@@ -16434,7 +16442,7 @@
         <v>177.25415102820591</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>11</v>
       </c>
@@ -16473,7 +16481,7 @@
         <v>163.91109373188704</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>11</v>
       </c>
@@ -16512,7 +16520,7 @@
         <v>152.37230172654765</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>11</v>
       </c>
@@ -16551,7 +16559,7 @@
         <v>140.024288415992</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>11</v>
       </c>
@@ -16590,7 +16598,7 @@
         <v>131.69818504810721</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>11</v>
       </c>
@@ -16629,7 +16637,7 @@
         <v>124.38939234296896</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>11</v>
       </c>
@@ -16668,7 +16676,7 @@
         <v>114.63898908250553</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>11</v>
       </c>
@@ -16707,7 +16715,7 @@
         <v>120.78151250834118</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>11</v>
       </c>
@@ -16746,7 +16754,7 @@
         <v>122.60026849077067</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>13</v>
       </c>
@@ -16785,7 +16793,7 @@
         <v>124.93667112323469</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>13</v>
       </c>
@@ -16824,7 +16832,7 @@
         <v>124.96779433612404</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>11</v>
       </c>
@@ -16863,7 +16871,7 @@
         <v>129.79199313700218</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>11</v>
       </c>
@@ -16902,7 +16910,7 @@
         <v>131.73065826932722</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>11</v>
       </c>
@@ -16941,7 +16949,7 @@
         <v>131.64595137047274</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -16980,7 +16988,7 @@
         <v>128.30423976627506</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>13</v>
       </c>
@@ -17019,7 +17027,7 @@
         <v>129.44047418407598</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -17058,7 +17066,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>11</v>
       </c>
@@ -17097,7 +17105,7 @@
         <v>130.70704467197089</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>11</v>
       </c>
@@ -17136,7 +17144,7 @@
         <v>128.48177134567464</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>11</v>
       </c>
@@ -17175,7 +17183,7 @@
         <v>128.10946048537377</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>11</v>
       </c>
@@ -17214,7 +17222,7 @@
         <v>124.8789550474776</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>11</v>
       </c>
@@ -17253,7 +17261,7 @@
         <v>121.50336624435865</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>11</v>
       </c>
@@ -17292,7 +17300,7 @@
         <v>122.61326843867039</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>11</v>
       </c>
@@ -17331,7 +17339,7 @@
         <v>125.23314149127367</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>13</v>
       </c>
@@ -17370,7 +17378,7 @@
         <v>126.58087530931341</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>13</v>
       </c>
@@ -17409,7 +17417,7 @@
         <v>129.34076490165924</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>13</v>
       </c>
@@ -17448,7 +17456,7 @@
         <v>130.00132062578234</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>11</v>
       </c>
@@ -17487,7 +17495,7 @@
         <v>130.20339223863886</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>11</v>
       </c>
@@ -17526,7 +17534,7 @@
         <v>130.75087634814548</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>11</v>
       </c>
@@ -17565,7 +17573,7 @@
         <v>131.73065826932722</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>11</v>
       </c>
@@ -17604,7 +17612,7 @@
         <v>128.44456733641957</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>11</v>
       </c>
@@ -17643,7 +17651,7 @@
         <v>121.88265566719532</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>11</v>
       </c>
@@ -17682,7 +17690,7 @@
         <v>114.9135881179733</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>11</v>
       </c>
@@ -17721,7 +17729,7 @@
         <v>105.31750321605139</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>11</v>
       </c>
@@ -17760,7 +17768,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>13</v>
       </c>
@@ -17799,7 +17807,7 @@
         <v>104.55715050076574</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>11</v>
       </c>
@@ -17838,7 +17846,7 @@
         <v>107.68350603875257</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>11</v>
       </c>
@@ -17877,7 +17885,7 @@
         <v>106.27577088362472</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>11</v>
       </c>
@@ -17916,7 +17924,7 @@
         <v>108.40740427208819</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>13</v>
       </c>
@@ -17955,7 +17963,7 @@
         <v>104.65124598397863</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>13</v>
       </c>
@@ -17994,7 +18002,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>11</v>
       </c>
@@ -18033,7 +18041,7 @@
         <v>107.2342511618268</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>11</v>
       </c>
@@ -18072,7 +18080,7 @@
         <v>106.70356790964144</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>11</v>
       </c>
@@ -18111,7 +18119,7 @@
         <v>104.06836380358112</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>11</v>
       </c>
@@ -18150,7 +18158,7 @@
         <v>108.48143449687807</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>11</v>
       </c>
@@ -18189,7 +18197,7 @@
         <v>109.70510453443482</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>11</v>
       </c>
@@ -18228,7 +18236,7 @@
         <v>110.94971006172204</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>11</v>
       </c>
@@ -18267,7 +18275,7 @@
         <v>124.29411050415683</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>11</v>
       </c>
@@ -18306,7 +18314,7 @@
         <v>-172.51086368259493</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>11</v>
       </c>
@@ -18345,7 +18353,7 @@
         <v>-143.27302153518156</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>11</v>
       </c>
@@ -18384,7 +18392,7 @@
         <v>-148.84967211426914</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>11</v>
       </c>
@@ -18423,7 +18431,7 @@
         <v>-164.93353472600882</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>11</v>
       </c>
@@ -18462,7 +18470,7 @@
         <v>-165.99793840377137</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>11</v>
       </c>
@@ -18501,7 +18509,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>11</v>
       </c>
@@ -18540,7 +18548,7 @@
         <v>160.48954548388298</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>11</v>
       </c>
@@ -18579,7 +18587,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>11</v>
       </c>
@@ -18618,7 +18626,7 @@
         <v>151.40227109485002</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>13</v>
       </c>
@@ -18657,7 +18665,7 @@
         <v>141.40245923045339</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>11</v>
       </c>
@@ -18696,7 +18704,7 @@
         <v>134.21092002689477</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>13</v>
       </c>
@@ -18735,7 +18743,7 @@
         <v>134.32727692420914</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>13</v>
       </c>
@@ -18774,7 +18782,7 @@
         <v>128.92547496703182</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>13</v>
       </c>
@@ -18813,7 +18821,7 @@
         <v>126.92266040132077</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>13</v>
       </c>
@@ -18852,7 +18860,7 @@
         <v>125.56971728725681</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>11</v>
       </c>
@@ -18891,7 +18899,7 @@
         <v>124.00086872687159</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>11</v>
       </c>
@@ -18930,7 +18938,7 @@
         <v>122.40964983573657</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>11</v>
       </c>
@@ -18969,7 +18977,7 @@
         <v>121.17402465560643</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>11</v>
       </c>
@@ -19008,7 +19016,7 @@
         <v>119.54336481719187</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>11</v>
       </c>
@@ -19047,7 +19055,7 @@
         <v>110.64223267779717</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>11</v>
       </c>
@@ -19086,7 +19094,7 @@
         <v>104.78272373063027</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>11</v>
       </c>
@@ -19125,7 +19133,7 @@
         <v>99.99478809391023</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>11</v>
       </c>
@@ -19164,7 +19172,7 @@
         <v>19.065659743904597</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>11</v>
       </c>
@@ -19203,7 +19211,7 @@
         <v>102.43378055985845</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>11</v>
       </c>
@@ -19242,7 +19250,7 @@
         <v>137.92919152148028</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>11</v>
       </c>

</xml_diff>